<commit_message>
Created a mess with config
Should it be global? Or should it be passed into every parameters? And
does this mean overloads for all the static methods? Yuck.
</commit_message>
<xml_diff>
--- a/BasicTypes/Dictionary/RawData.xlsx
+++ b/BasicTypes/Dictionary/RawData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="658">
   <si>
     <t>a</t>
   </si>
@@ -75,9 +75,6 @@
     <t>not</t>
   </si>
   <si>
-    <t>ne, neniu</t>
-  </si>
-  <si>
     <t>nenio, neado, nul</t>
   </si>
   <si>
@@ -1879,6 +1876,120 @@
   </si>
   <si>
     <t>conditional</t>
+  </si>
+  <si>
+    <t>ne</t>
+  </si>
+  <si>
+    <t>completely, wholely</t>
+  </si>
+  <si>
+    <t>tute, komplete</t>
+  </si>
+  <si>
+    <t>differently</t>
+  </si>
+  <si>
+    <t>alie, malsame </t>
+  </si>
+  <si>
+    <t>lowly</t>
+  </si>
+  <si>
+    <t>malsupre, sube</t>
+  </si>
+  <si>
+    <t>permanently</t>
+  </si>
+  <si>
+    <t>daŭre</t>
+  </si>
+  <si>
+    <t>badly, negatively, wrongly, evilly, overly complex, unhealthyly</t>
+  </si>
+  <si>
+    <t>malbone, aĉe, malĝuste, malice, tro komplekse,  malsane</t>
+  </si>
+  <si>
+    <t>internally</t>
+  </si>
+  <si>
+    <t>ene, interne</t>
+  </si>
+  <si>
+    <t>dirtily, grossly, filthily</t>
+  </si>
+  <si>
+    <t>malpure, naŭze</t>
+  </si>
+  <si>
+    <t>humanly,  personally</t>
+  </si>
+  <si>
+    <t>home,  persone</t>
+  </si>
+  <si>
+    <t>solidly</t>
+  </si>
+  <si>
+    <t>malmole, solide</t>
+  </si>
+  <si>
+    <t>colourfully</t>
+  </si>
+  <si>
+    <t>kolore, bunte</t>
+  </si>
+  <si>
+    <t>audibly</t>
+  </si>
+  <si>
+    <t>aŭde, aŭskulte</t>
+  </si>
+  <si>
+    <t>communally, publicly</t>
+  </si>
+  <si>
+    <t>komune, publike, socie</t>
+  </si>
+  <si>
+    <t>dorma, ripoza</t>
+  </si>
+  <si>
+    <t>sleepily</t>
+  </si>
+  <si>
+    <t>dorme, ripoze</t>
+  </si>
+  <si>
+    <t>mainly</t>
+  </si>
+  <si>
+    <t>ĉefe, estre</t>
+  </si>
+  <si>
+    <t>coldly</t>
+  </si>
+  <si>
+    <t>malvarme, fride</t>
+  </si>
+  <si>
+    <t>little, a bit, less</t>
+  </si>
+  <si>
+    <t>iomete, malmulte, malpli</t>
+  </si>
+  <si>
+    <t>visually</t>
+  </si>
+  <si>
+    <t>vide</t>
+  </si>
+  <si>
+    <t>maternally, fatherly</t>
+  </si>
+  <si>
+    <t>gepatre, patre, patrine</t>
   </si>
 </sst>
 </file>
@@ -2248,8 +2359,8 @@
   <dimension ref="A1:N251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2275,34 +2386,34 @@
         <v>16</v>
       </c>
       <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
         <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>24</v>
       </c>
       <c r="G1" t="s">
         <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="L1" t="s">
         <v>2</v>
       </c>
       <c r="M1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2377,13 +2488,16 @@
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="G7" t="s">
+        <v>620</v>
+      </c>
+      <c r="L7" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -2391,10 +2505,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -2402,10 +2516,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -2413,13 +2527,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
+      <c r="G10" s="1" t="s">
+        <v>621</v>
       </c>
       <c r="N10" s="3"/>
     </row>
@@ -2428,13 +2545,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>31</v>
+      <c r="G11" s="2" t="s">
+        <v>622</v>
       </c>
       <c r="N11" s="3"/>
     </row>
@@ -2443,13 +2563,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
+      <c r="G12" s="1" t="s">
+        <v>621</v>
       </c>
       <c r="N12" s="3"/>
     </row>
@@ -2458,13 +2581,16 @@
         <v>7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>31</v>
+      <c r="G13" s="2" t="s">
+        <v>622</v>
       </c>
       <c r="N13" s="3"/>
     </row>
@@ -2473,22 +2599,25 @@
         <v>5</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" t="s">
         <v>33</v>
       </c>
-      <c r="D14" t="s">
-        <v>34</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
+        <v>623</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="M14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N14" s="3"/>
     </row>
@@ -2497,22 +2626,25 @@
         <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>624</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="M15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N15" s="3"/>
     </row>
@@ -2521,13 +2653,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="M16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N16" s="3"/>
     </row>
@@ -2536,13 +2668,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="M17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N17" s="3"/>
     </row>
@@ -2551,13 +2683,16 @@
         <v>5</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>612</v>
+      <c r="G18" s="1" t="s">
+        <v>625</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -2570,13 +2705,16 @@
         <v>7</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>614</v>
+      <c r="G19" s="2" t="s">
+        <v>626</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -2589,16 +2727,19 @@
         <v>5</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>47</v>
+      <c r="G20" s="1" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -2606,16 +2747,19 @@
         <v>7</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -2623,10 +2767,10 @@
         <v>5</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -2634,10 +2778,10 @@
         <v>7</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -2648,7 +2792,7 @@
         <v>5</v>
       </c>
       <c r="M24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -2659,7 +2803,7 @@
         <v>5</v>
       </c>
       <c r="M25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -2667,10 +2811,10 @@
         <v>5</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -2678,10 +2822,10 @@
         <v>7</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -2689,7 +2833,7 @@
         <v>5</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -2697,7 +2841,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -2705,22 +2849,25 @@
         <v>5</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="F30" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="L30" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -2728,22 +2875,25 @@
         <v>7</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="F31" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="L31" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -2751,10 +2901,10 @@
         <v>5</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -2762,10 +2912,10 @@
         <v>7</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2773,13 +2923,16 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" t="s">
         <v>75</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>76</v>
       </c>
-      <c r="D34" t="s">
-        <v>77</v>
+      <c r="G34" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2787,13 +2940,16 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" t="s">
         <v>78</v>
       </c>
-      <c r="D35" t="s">
-        <v>79</v>
+      <c r="G35" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -2801,19 +2957,22 @@
         <v>5</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" t="s">
         <v>86</v>
       </c>
-      <c r="D36" t="s">
-        <v>87</v>
-      </c>
       <c r="E36" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" t="s">
+        <v>633</v>
+      </c>
+      <c r="L36" t="s">
         <v>84</v>
-      </c>
-      <c r="L36" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -2821,19 +2980,22 @@
         <v>7</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" t="s">
         <v>82</v>
       </c>
-      <c r="D37" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" t="s">
-        <v>83</v>
+      <c r="G37" t="s">
+        <v>634</v>
       </c>
       <c r="L37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -2841,19 +3003,22 @@
         <v>5</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" t="s">
         <v>89</v>
       </c>
-      <c r="C38" t="s">
-        <v>90</v>
-      </c>
       <c r="D38" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" t="s">
         <v>93</v>
       </c>
-      <c r="E38" t="s">
-        <v>94</v>
+      <c r="G38" t="s">
+        <v>635</v>
       </c>
       <c r="I38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -2861,16 +3026,19 @@
         <v>7</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" t="s">
         <v>95</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>96</v>
       </c>
-      <c r="E39" t="s">
-        <v>97</v>
+      <c r="G39" t="s">
+        <v>636</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2878,10 +3046,10 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" t="s">
         <v>98</v>
-      </c>
-      <c r="D40" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2889,10 +3057,10 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -2900,13 +3068,13 @@
         <v>5</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" t="s">
         <v>101</v>
-      </c>
-      <c r="C42" t="s">
-        <v>103</v>
-      </c>
-      <c r="E42" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -2914,13 +3082,13 @@
         <v>7</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C43" t="s">
+        <v>104</v>
+      </c>
+      <c r="E43" t="s">
         <v>105</v>
-      </c>
-      <c r="E43" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -2928,10 +3096,10 @@
         <v>5</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" t="s">
         <v>107</v>
-      </c>
-      <c r="C44" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -2939,10 +3107,10 @@
         <v>7</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -2950,16 +3118,16 @@
         <v>5</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E46" t="s">
+        <v>113</v>
+      </c>
+      <c r="F46" t="s">
         <v>114</v>
-      </c>
-      <c r="F46" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -2967,16 +3135,16 @@
         <v>7</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C47" t="s">
+        <v>110</v>
+      </c>
+      <c r="E47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F47" t="s">
         <v>111</v>
-      </c>
-      <c r="E47" t="s">
-        <v>113</v>
-      </c>
-      <c r="F47" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -2984,19 +3152,19 @@
         <v>5</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C48" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" t="s">
         <v>118</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
+        <v>116</v>
+      </c>
+      <c r="F48" t="s">
         <v>119</v>
-      </c>
-      <c r="E48" t="s">
-        <v>117</v>
-      </c>
-      <c r="F48" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3004,19 +3172,19 @@
         <v>7</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C49" t="s">
+        <v>121</v>
+      </c>
+      <c r="D49" t="s">
         <v>122</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F49" t="s">
         <v>123</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F49" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3024,10 +3192,10 @@
         <v>5</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C50" t="s">
         <v>125</v>
-      </c>
-      <c r="C50" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3035,10 +3203,10 @@
         <v>7</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3046,19 +3214,19 @@
         <v>5</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" t="s">
+        <v>129</v>
+      </c>
+      <c r="E52" t="s">
         <v>128</v>
       </c>
-      <c r="C52" t="s">
+      <c r="F52" t="s">
         <v>130</v>
       </c>
-      <c r="E52" t="s">
-        <v>129</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="K52" t="s">
         <v>131</v>
-      </c>
-      <c r="K52" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3066,19 +3234,19 @@
         <v>7</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C53" t="s">
+        <v>133</v>
+      </c>
+      <c r="E53" t="s">
+        <v>132</v>
+      </c>
+      <c r="F53" t="s">
         <v>134</v>
       </c>
-      <c r="E53" t="s">
-        <v>133</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="K53" t="s">
         <v>135</v>
-      </c>
-      <c r="K53" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -3086,13 +3254,13 @@
         <v>5</v>
       </c>
       <c r="B54" t="s">
+        <v>136</v>
+      </c>
+      <c r="E54" t="s">
         <v>137</v>
       </c>
-      <c r="E54" t="s">
+      <c r="H54" t="s">
         <v>138</v>
-      </c>
-      <c r="H54" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -3100,13 +3268,13 @@
         <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3114,10 +3282,10 @@
         <v>5</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C56" t="s">
         <v>143</v>
-      </c>
-      <c r="C56" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3125,10 +3293,10 @@
         <v>7</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C57" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3136,10 +3304,13 @@
         <v>5</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3147,13 +3318,16 @@
         <v>7</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="G59" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K59" t="s">
         <v>148</v>
-      </c>
-      <c r="K59" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3161,10 +3335,10 @@
         <v>5</v>
       </c>
       <c r="B60" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D60" t="s">
         <v>150</v>
-      </c>
-      <c r="D60" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3172,10 +3346,10 @@
         <v>7</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3183,13 +3357,16 @@
         <v>5</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C62" t="s">
+        <v>153</v>
+      </c>
+      <c r="D62" t="s">
         <v>152</v>
       </c>
-      <c r="C62" t="s">
-        <v>154</v>
-      </c>
-      <c r="D62" t="s">
-        <v>153</v>
+      <c r="G62" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3197,13 +3374,16 @@
         <v>7</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D63" t="s">
-        <v>155</v>
+        <v>154</v>
+      </c>
+      <c r="G63" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3211,10 +3391,10 @@
         <v>5</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3222,10 +3402,10 @@
         <v>7</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3233,13 +3413,13 @@
         <v>5</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3247,13 +3427,13 @@
         <v>7</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C67" t="s">
+        <v>162</v>
+      </c>
+      <c r="D67" t="s">
         <v>163</v>
-      </c>
-      <c r="D67" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3261,16 +3441,19 @@
         <v>5</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C68" t="s">
         <v>165</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>166</v>
       </c>
-      <c r="D68" t="s">
-        <v>167</v>
-      </c>
       <c r="E68" t="s">
-        <v>166</v>
+        <v>165</v>
+      </c>
+      <c r="G68" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3278,16 +3461,19 @@
         <v>7</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C69" t="s">
+        <v>167</v>
+      </c>
+      <c r="D69" t="s">
         <v>168</v>
       </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>169</v>
       </c>
-      <c r="E69" t="s">
-        <v>170</v>
+      <c r="G69" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3295,13 +3481,16 @@
         <v>5</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D70" t="s">
+        <v>172</v>
+      </c>
+      <c r="E70" t="s">
         <v>171</v>
       </c>
-      <c r="D70" t="s">
-        <v>173</v>
-      </c>
-      <c r="E70" t="s">
-        <v>172</v>
+      <c r="G70" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3309,13 +3498,16 @@
         <v>7</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D71" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E71" t="s">
-        <v>174</v>
+        <v>173</v>
+      </c>
+      <c r="G71" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3323,13 +3515,16 @@
         <v>5</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C72" t="s">
+        <v>175</v>
+      </c>
+      <c r="D72" t="s">
         <v>176</v>
       </c>
-      <c r="D72" t="s">
-        <v>177</v>
+      <c r="G72" t="s">
+        <v>643</v>
       </c>
     </row>
     <row r="73" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3337,13 +3532,16 @@
         <v>7</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C73" t="s">
+        <v>177</v>
+      </c>
+      <c r="D73" t="s">
         <v>178</v>
       </c>
-      <c r="D73" t="s">
-        <v>179</v>
+      <c r="G73" t="s">
+        <v>644</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3351,10 +3549,10 @@
         <v>5</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N74" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3362,10 +3560,10 @@
         <v>7</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N75" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="76" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3373,16 +3571,19 @@
         <v>5</v>
       </c>
       <c r="B76" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C76" t="s">
         <v>182</v>
       </c>
-      <c r="C76" t="s">
-        <v>183</v>
-      </c>
       <c r="D76" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F76" t="s">
-        <v>183</v>
+        <v>182</v>
+      </c>
+      <c r="G76" t="s">
+        <v>646</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3390,13 +3591,19 @@
         <v>7</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C77" t="s">
-        <v>186</v>
+        <v>185</v>
+      </c>
+      <c r="D77" t="s">
+        <v>645</v>
       </c>
       <c r="F77" t="s">
-        <v>184</v>
+        <v>183</v>
+      </c>
+      <c r="G77" t="s">
+        <v>647</v>
       </c>
     </row>
     <row r="78" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3404,10 +3611,10 @@
         <v>5</v>
       </c>
       <c r="B78" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3415,10 +3622,10 @@
         <v>7</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="80" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3426,16 +3633,19 @@
         <v>5</v>
       </c>
       <c r="B80" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="D80" t="s">
         <v>191</v>
       </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>192</v>
       </c>
-      <c r="E80" t="s">
-        <v>193</v>
+      <c r="G80" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3443,16 +3653,19 @@
         <v>7</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C81" t="s">
+        <v>193</v>
+      </c>
+      <c r="D81" t="s">
         <v>194</v>
       </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>195</v>
       </c>
-      <c r="E81" t="s">
-        <v>196</v>
+      <c r="G81" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3460,10 +3673,10 @@
         <v>5</v>
       </c>
       <c r="B82" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C82" t="s">
         <v>197</v>
-      </c>
-      <c r="C82" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3471,10 +3684,10 @@
         <v>7</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3482,16 +3695,19 @@
         <v>5</v>
       </c>
       <c r="B84" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C84" t="s">
         <v>200</v>
       </c>
-      <c r="C84" t="s">
-        <v>201</v>
-      </c>
       <c r="D84" t="s">
+        <v>202</v>
+      </c>
+      <c r="E84" t="s">
         <v>203</v>
       </c>
-      <c r="E84" t="s">
-        <v>204</v>
+      <c r="G84" t="s">
+        <v>650</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3499,16 +3715,19 @@
         <v>7</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C85" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D85" t="s">
+        <v>204</v>
+      </c>
+      <c r="E85" t="s">
         <v>205</v>
       </c>
-      <c r="E85" t="s">
-        <v>206</v>
+      <c r="G85" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3516,7 +3735,7 @@
         <v>5</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3524,7 +3743,7 @@
         <v>7</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3532,13 +3751,16 @@
         <v>5</v>
       </c>
       <c r="B88" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D88" t="s">
         <v>208</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>209</v>
       </c>
-      <c r="E88" t="s">
-        <v>210</v>
+      <c r="G88" t="s">
+        <v>652</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3546,13 +3768,16 @@
         <v>7</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D89" t="s">
+        <v>210</v>
+      </c>
+      <c r="E89" t="s">
         <v>211</v>
       </c>
-      <c r="E89" t="s">
-        <v>212</v>
+      <c r="G89" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3560,10 +3785,10 @@
         <v>5</v>
       </c>
       <c r="B90" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C90" t="s">
         <v>213</v>
-      </c>
-      <c r="C90" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3571,10 +3796,10 @@
         <v>7</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C91" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="33" x14ac:dyDescent="0.25">
@@ -3582,10 +3807,10 @@
         <v>5</v>
       </c>
       <c r="B92" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C92" s="4" t="s">
         <v>216</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3593,10 +3818,10 @@
         <v>7</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3604,10 +3829,10 @@
         <v>5</v>
       </c>
       <c r="B94" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D94" t="s">
         <v>219</v>
-      </c>
-      <c r="D94" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3615,10 +3840,10 @@
         <v>7</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D95" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -3626,13 +3851,13 @@
         <v>5</v>
       </c>
       <c r="B96" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="H96" s="1" t="s">
         <v>615</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>617</v>
-      </c>
-      <c r="H96" s="1" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -3640,13 +3865,13 @@
         <v>7</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -3654,10 +3879,10 @@
         <v>5</v>
       </c>
       <c r="B98" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C98" t="s">
         <v>222</v>
-      </c>
-      <c r="C98" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -3665,10 +3890,10 @@
         <v>7</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C99" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -3676,16 +3901,19 @@
         <v>5</v>
       </c>
       <c r="B100" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D100" t="s">
+        <v>227</v>
+      </c>
+      <c r="E100" t="s">
         <v>225</v>
       </c>
-      <c r="D100" t="s">
-        <v>228</v>
-      </c>
-      <c r="E100" t="s">
+      <c r="F100" t="s">
         <v>226</v>
       </c>
-      <c r="F100" t="s">
-        <v>227</v>
+      <c r="G100" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -3693,16 +3921,19 @@
         <v>7</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D101" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E101" t="s">
+        <v>228</v>
+      </c>
+      <c r="F101" t="s">
         <v>229</v>
       </c>
-      <c r="F101" t="s">
-        <v>230</v>
+      <c r="G101" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -3710,10 +3941,10 @@
         <v>5</v>
       </c>
       <c r="B102" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -3721,10 +3952,10 @@
         <v>7</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="33" x14ac:dyDescent="0.25">
@@ -3732,10 +3963,10 @@
         <v>5</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -3743,10 +3974,10 @@
         <v>7</v>
       </c>
       <c r="B105" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -3754,13 +3985,16 @@
         <v>5</v>
       </c>
       <c r="B106" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="D106" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D106" s="1" t="s">
-        <v>240</v>
+      <c r="G106" s="1" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -3768,35 +4002,38 @@
         <v>7</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C107" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D107" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="G107" s="2" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>5</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" ht="33" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>5</v>
-      </c>
-      <c r="B108" s="3" t="s">
+      <c r="C108" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C108" s="1" t="s">
+    </row>
+    <row r="109" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>7</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C109" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>7</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -3804,13 +4041,13 @@
         <v>5</v>
       </c>
       <c r="B110" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="D110" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -3818,13 +4055,13 @@
         <v>7</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C111" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D111" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -3832,16 +4069,16 @@
         <v>5</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C112" t="s">
+        <v>253</v>
+      </c>
+      <c r="D112" t="s">
         <v>254</v>
       </c>
-      <c r="D112" t="s">
-        <v>255</v>
-      </c>
       <c r="I112" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="113" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -3849,13 +4086,13 @@
         <v>7</v>
       </c>
       <c r="B113" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="D113" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="114" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -3863,13 +4100,13 @@
         <v>5</v>
       </c>
       <c r="B114" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C114" t="s">
         <v>256</v>
       </c>
-      <c r="C114" t="s">
+      <c r="D114" t="s">
         <v>257</v>
-      </c>
-      <c r="D114" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="115" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -3877,13 +4114,13 @@
         <v>7</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C115" t="s">
+        <v>258</v>
+      </c>
+      <c r="D115" t="s">
         <v>259</v>
-      </c>
-      <c r="D115" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="116" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -3891,13 +4128,13 @@
         <v>5</v>
       </c>
       <c r="B116" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C116" t="s">
         <v>261</v>
       </c>
-      <c r="C116" t="s">
+      <c r="E116" t="s">
         <v>262</v>
-      </c>
-      <c r="E116" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="117" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -3905,13 +4142,13 @@
         <v>7</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C117" t="s">
+        <v>263</v>
+      </c>
+      <c r="E117" t="s">
         <v>264</v>
-      </c>
-      <c r="E117" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="118" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -3919,19 +4156,19 @@
         <v>5</v>
       </c>
       <c r="B118" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C118" t="s">
         <v>266</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
+        <v>269</v>
+      </c>
+      <c r="E118" t="s">
+        <v>268</v>
+      </c>
+      <c r="F118" t="s">
         <v>267</v>
-      </c>
-      <c r="D118" t="s">
-        <v>270</v>
-      </c>
-      <c r="E118" t="s">
-        <v>269</v>
-      </c>
-      <c r="F118" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="119" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -3939,19 +4176,19 @@
         <v>7</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C119" t="s">
+        <v>270</v>
+      </c>
+      <c r="D119" t="s">
+        <v>272</v>
+      </c>
+      <c r="E119" t="s">
+        <v>273</v>
+      </c>
+      <c r="F119" t="s">
         <v>271</v>
-      </c>
-      <c r="D119" t="s">
-        <v>273</v>
-      </c>
-      <c r="E119" t="s">
-        <v>274</v>
-      </c>
-      <c r="F119" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="120" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -3959,13 +4196,13 @@
         <v>5</v>
       </c>
       <c r="B120" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="121" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -3973,13 +4210,13 @@
         <v>7</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C121" t="s">
+        <v>277</v>
+      </c>
+      <c r="D121" t="s">
         <v>278</v>
-      </c>
-      <c r="D121" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="122" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -3987,10 +4224,10 @@
         <v>5</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L122" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="123" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -3998,10 +4235,10 @@
         <v>7</v>
       </c>
       <c r="B123" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="L123" t="s">
         <v>280</v>
-      </c>
-      <c r="L123" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="124" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4009,13 +4246,13 @@
         <v>5</v>
       </c>
       <c r="B124" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C124" t="s">
         <v>283</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D124" t="s">
         <v>284</v>
-      </c>
-      <c r="D124" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="125" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4023,13 +4260,13 @@
         <v>7</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C125" t="s">
+        <v>285</v>
+      </c>
+      <c r="D125" t="s">
         <v>286</v>
-      </c>
-      <c r="D125" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="126" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4037,19 +4274,19 @@
         <v>5</v>
       </c>
       <c r="B126" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C126" t="s">
         <v>288</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" t="s">
         <v>289</v>
       </c>
-      <c r="D126" t="s">
+      <c r="E126" t="s">
+        <v>291</v>
+      </c>
+      <c r="F126" t="s">
         <v>290</v>
-      </c>
-      <c r="E126" t="s">
-        <v>292</v>
-      </c>
-      <c r="F126" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="127" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4057,19 +4294,19 @@
         <v>7</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C127" t="s">
+        <v>292</v>
+      </c>
+      <c r="D127" t="s">
         <v>293</v>
       </c>
-      <c r="D127" t="s">
+      <c r="E127" t="s">
+        <v>295</v>
+      </c>
+      <c r="F127" t="s">
         <v>294</v>
-      </c>
-      <c r="E127" t="s">
-        <v>296</v>
-      </c>
-      <c r="F127" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="128" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4077,16 +4314,16 @@
         <v>5</v>
       </c>
       <c r="B128" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C128" t="s">
+        <v>298</v>
+      </c>
+      <c r="D128" t="s">
         <v>297</v>
       </c>
-      <c r="C128" t="s">
+      <c r="E128" t="s">
         <v>299</v>
-      </c>
-      <c r="D128" t="s">
-        <v>298</v>
-      </c>
-      <c r="E128" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4094,16 +4331,16 @@
         <v>7</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C129" t="s">
+        <v>301</v>
+      </c>
+      <c r="D129" t="s">
+        <v>300</v>
+      </c>
+      <c r="E129" t="s">
         <v>302</v>
-      </c>
-      <c r="D129" t="s">
-        <v>301</v>
-      </c>
-      <c r="E129" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4111,10 +4348,10 @@
         <v>5</v>
       </c>
       <c r="B130" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C130" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4122,7 +4359,7 @@
         <v>7</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4130,10 +4367,10 @@
         <v>5</v>
       </c>
       <c r="B132" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C132" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4141,10 +4378,10 @@
         <v>7</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="33" x14ac:dyDescent="0.25">
@@ -4152,13 +4389,13 @@
         <v>5</v>
       </c>
       <c r="B134" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D134" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="D134" s="4" t="s">
+      <c r="E134" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4166,13 +4403,13 @@
         <v>7</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D135" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E135" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="E135" s="2" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4180,10 +4417,10 @@
         <v>5</v>
       </c>
       <c r="B136" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4191,10 +4428,10 @@
         <v>7</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4202,10 +4439,10 @@
         <v>5</v>
       </c>
       <c r="B138" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C138" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4213,10 +4450,10 @@
         <v>7</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4224,10 +4461,10 @@
         <v>5</v>
       </c>
       <c r="B140" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D140" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4235,10 +4472,10 @@
         <v>7</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4246,10 +4483,10 @@
         <v>5</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4257,10 +4494,10 @@
         <v>7</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -4268,10 +4505,10 @@
         <v>5</v>
       </c>
       <c r="B144" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C144" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="145" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4279,10 +4516,10 @@
         <v>7</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="146" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4290,13 +4527,13 @@
         <v>5</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L146" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N146" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="147" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4304,13 +4541,13 @@
         <v>7</v>
       </c>
       <c r="B147" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="L147" t="s">
         <v>329</v>
       </c>
-      <c r="L147" t="s">
-        <v>330</v>
-      </c>
       <c r="N147" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="148" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4318,10 +4555,10 @@
         <v>5</v>
       </c>
       <c r="B148" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C148" t="s">
         <v>332</v>
-      </c>
-      <c r="C148" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="149" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4329,10 +4566,10 @@
         <v>7</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C149" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="150" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4340,16 +4577,16 @@
         <v>5</v>
       </c>
       <c r="B150" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C150" t="s">
         <v>335</v>
       </c>
-      <c r="C150" t="s">
+      <c r="D150" t="s">
+        <v>335</v>
+      </c>
+      <c r="E150" t="s">
         <v>336</v>
-      </c>
-      <c r="D150" t="s">
-        <v>336</v>
-      </c>
-      <c r="E150" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="151" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4357,16 +4594,16 @@
         <v>7</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C151" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D151" t="s">
+        <v>337</v>
+      </c>
+      <c r="E151" t="s">
         <v>338</v>
-      </c>
-      <c r="E151" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="152" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4374,16 +4611,16 @@
         <v>5</v>
       </c>
       <c r="B152" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="I152" t="s">
         <v>340</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="I152" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="153" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4391,13 +4628,13 @@
         <v>7</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C153" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D153" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="D153" s="2" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="154" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4405,10 +4642,10 @@
         <v>5</v>
       </c>
       <c r="B154" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="E154" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="155" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4416,10 +4653,10 @@
         <v>7</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="156" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4427,19 +4664,19 @@
         <v>5</v>
       </c>
       <c r="B156" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C156" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="E156" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="E156" s="1" t="s">
+      <c r="F156" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="F156" s="1" t="s">
+      <c r="L156" s="4" t="s">
         <v>352</v>
-      </c>
-      <c r="L156" s="4" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="157" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4447,19 +4684,19 @@
         <v>7</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C157" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="F157" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="E157" s="2" t="s">
+      <c r="L157" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="F157" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="L157" s="2" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="158" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4467,19 +4704,19 @@
         <v>5</v>
       </c>
       <c r="B158" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C158" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C158" s="1" t="s">
+      <c r="D158" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="D158" s="1" t="s">
+      <c r="E158" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="E158" s="1" t="s">
+      <c r="F158" s="1" t="s">
         <v>361</v>
-      </c>
-      <c r="F158" s="1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="159" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4487,19 +4724,19 @@
         <v>7</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C159" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D159" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="D159" s="2" t="s">
+      <c r="E159" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="E159" s="2" t="s">
+      <c r="F159" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="F159" s="2" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="160" spans="1:14" ht="33" x14ac:dyDescent="0.25">
@@ -4507,10 +4744,10 @@
         <v>5</v>
       </c>
       <c r="B160" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C160" s="4" t="s">
         <v>367</v>
-      </c>
-      <c r="C160" s="4" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="161" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4518,10 +4755,10 @@
         <v>7</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="162" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4529,10 +4766,10 @@
         <v>5</v>
       </c>
       <c r="B162" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="C162" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="C162" s="1" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="163" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4540,10 +4777,10 @@
         <v>7</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C163" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="164" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4551,13 +4788,13 @@
         <v>5</v>
       </c>
       <c r="B164" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E164" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="165" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4565,13 +4802,13 @@
         <v>7</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="166" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4579,10 +4816,10 @@
         <v>5</v>
       </c>
       <c r="B166" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="C166" t="s">
         <v>377</v>
-      </c>
-      <c r="C166" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="167" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4590,10 +4827,10 @@
         <v>7</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C167" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="168" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4601,10 +4838,10 @@
         <v>5</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="N168" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="169" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4612,7 +4849,7 @@
         <v>7</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="170" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4620,16 +4857,16 @@
         <v>5</v>
       </c>
       <c r="B170" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="C170" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="C170" s="1" t="s">
+      <c r="E170" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="F170" t="s">
         <v>381</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="F170" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="171" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4637,16 +4874,16 @@
         <v>7</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C171" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F171" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="E171" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="F171" s="2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="172" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4654,16 +4891,16 @@
         <v>5</v>
       </c>
       <c r="B172" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D172" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="C172" s="1" t="s">
+      <c r="E172" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="173" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4671,16 +4908,16 @@
         <v>7</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C173" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D173" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E173" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="D173" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="E173" s="2" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="174" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4688,16 +4925,16 @@
         <v>5</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C174" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="D174" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="D174" s="1" t="s">
+      <c r="E174" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="175" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4705,16 +4942,16 @@
         <v>7</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C175" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="D175" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="D175" s="2" t="s">
+      <c r="E175" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="E175" s="2" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="176" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4722,10 +4959,10 @@
         <v>5</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C176" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="177" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4733,10 +4970,10 @@
         <v>7</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C177" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="178" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4744,16 +4981,16 @@
         <v>5</v>
       </c>
       <c r="B178" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H178" s="1" t="s">
         <v>404</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="H178" s="1" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="179" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4761,16 +4998,16 @@
         <v>7</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C179" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="D179" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="H179" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="D179" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="H179" s="2" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="180" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4778,10 +5015,10 @@
         <v>5</v>
       </c>
       <c r="B180" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="C180" t="s">
         <v>411</v>
-      </c>
-      <c r="C180" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="181" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4789,10 +5026,10 @@
         <v>7</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C181" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="182" spans="1:12" ht="33" x14ac:dyDescent="0.25">
@@ -4800,19 +5037,19 @@
         <v>5</v>
       </c>
       <c r="B182" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C182" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C182" s="1" t="s">
+      <c r="D182" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="D182" s="1" t="s">
+      <c r="E182" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="L182" s="4" t="s">
         <v>416</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="L182" s="4" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="183" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4820,19 +5057,19 @@
         <v>7</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C183" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D183" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="D183" s="2" t="s">
+      <c r="E183" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="L183" s="2" t="s">
         <v>420</v>
-      </c>
-      <c r="E183" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="L183" s="2" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="184" spans="1:12" ht="33" x14ac:dyDescent="0.25">
@@ -4840,13 +5077,13 @@
         <v>5</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C184" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="H184" s="1" t="s">
         <v>606</v>
-      </c>
-      <c r="H184" s="1" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="185" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4854,13 +5091,13 @@
         <v>7</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C185" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="H185" s="2" t="s">
         <v>608</v>
-      </c>
-      <c r="H185" s="2" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="186" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4868,16 +5105,16 @@
         <v>5</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C186" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D186" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="D186" s="1" t="s">
+      <c r="E186" s="1" t="s">
         <v>601</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="187" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4885,16 +5122,16 @@
         <v>7</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C187" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="D187" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="D187" s="2" t="s">
+      <c r="E187" s="2" t="s">
         <v>604</v>
-      </c>
-      <c r="E187" s="2" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="188" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4902,10 +5139,10 @@
         <v>5</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="189" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4913,10 +5150,10 @@
         <v>7</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="190" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4924,10 +5161,10 @@
         <v>5</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I190" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="191" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4935,10 +5172,10 @@
         <v>7</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I191" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="192" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4946,13 +5183,13 @@
         <v>5</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C192" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="D192" s="1" t="s">
         <v>592</v>
-      </c>
-      <c r="D192" s="1" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="193" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -4960,13 +5197,13 @@
         <v>7</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C193" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="D193" s="2" t="s">
         <v>594</v>
-      </c>
-      <c r="D193" s="2" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="194" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -4974,10 +5211,10 @@
         <v>5</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="195" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -4985,10 +5222,10 @@
         <v>7</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="196" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -4996,13 +5233,13 @@
         <v>5</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C196" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="D196" s="1" t="s">
         <v>586</v>
-      </c>
-      <c r="D196" s="1" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="197" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -5010,13 +5247,13 @@
         <v>7</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C197" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="D197" s="2" t="s">
         <v>588</v>
-      </c>
-      <c r="D197" s="2" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="198" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -5024,13 +5261,13 @@
         <v>5</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D198" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="E198" s="1" t="s">
         <v>582</v>
-      </c>
-      <c r="E198" s="1" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="199" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -5038,13 +5275,13 @@
         <v>7</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D199" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="E199" s="2" t="s">
         <v>584</v>
-      </c>
-      <c r="E199" s="2" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="200" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -5052,16 +5289,16 @@
         <v>5</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C200" t="s">
+        <v>578</v>
+      </c>
+      <c r="D200" t="s">
         <v>579</v>
       </c>
-      <c r="D200" t="s">
-        <v>580</v>
-      </c>
       <c r="I200" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="201" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -5069,16 +5306,16 @@
         <v>7</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C201" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D201" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I201" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="202" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -5086,10 +5323,10 @@
         <v>5</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="203" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -5097,10 +5334,10 @@
         <v>7</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="204" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -5108,13 +5345,13 @@
         <v>5</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C204" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="E204" s="1" t="s">
         <v>573</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="205" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -5122,13 +5359,13 @@
         <v>7</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C205" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="E205" s="2" t="s">
         <v>575</v>
-      </c>
-      <c r="E205" s="2" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="206" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -5136,19 +5373,19 @@
         <v>5</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C206" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="E206" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="E206" s="1" t="s">
+      <c r="F206" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="F206" s="1" t="s">
+      <c r="J206" s="1" t="s">
         <v>567</v>
-      </c>
-      <c r="J206" s="1" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="207" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -5156,19 +5393,19 @@
         <v>7</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C207" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="E207" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="E207" s="2" t="s">
+      <c r="F207" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="F207" s="2" t="s">
+      <c r="J207" s="2" t="s">
         <v>571</v>
-      </c>
-      <c r="J207" s="2" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="208" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -5176,10 +5413,10 @@
         <v>5</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="209" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5187,10 +5424,10 @@
         <v>7</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="210" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5198,16 +5435,16 @@
         <v>5</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C210" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D210" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="E210" s="1" t="s">
         <v>557</v>
-      </c>
-      <c r="E210" s="1" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="211" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5215,16 +5452,16 @@
         <v>7</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D211" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="E211" s="2" t="s">
         <v>560</v>
-      </c>
-      <c r="E211" s="2" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="212" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5232,10 +5469,10 @@
         <v>5</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="213" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5243,10 +5480,10 @@
         <v>7</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C213" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="214" spans="1:13" ht="33" x14ac:dyDescent="0.25">
@@ -5254,10 +5491,10 @@
         <v>5</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="215" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5265,10 +5502,10 @@
         <v>7</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="216" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5276,16 +5513,16 @@
         <v>5</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C216" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D216" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="D216" s="1" t="s">
+      <c r="E216" s="1" t="s">
         <v>548</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="217" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5293,16 +5530,16 @@
         <v>7</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C217" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="D217" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="D217" s="2" t="s">
+      <c r="E217" s="2" t="s">
         <v>551</v>
-      </c>
-      <c r="E217" s="2" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="218" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5310,13 +5547,13 @@
         <v>5</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H218" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="219" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5324,13 +5561,13 @@
         <v>7</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="H219" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="220" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5338,13 +5575,13 @@
         <v>5</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D220" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="M220" t="s">
         <v>539</v>
-      </c>
-      <c r="M220" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="221" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5352,13 +5589,13 @@
         <v>7</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D221" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="M221" t="s">
         <v>541</v>
-      </c>
-      <c r="M221" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="222" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5366,22 +5603,22 @@
         <v>5</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C222" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="D222" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="D222" s="1" t="s">
+      <c r="E222" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="E222" s="1" t="s">
-        <v>533</v>
-      </c>
       <c r="F222" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H222" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="223" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5389,22 +5626,22 @@
         <v>7</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C223" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="D223" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="D223" s="2" t="s">
+      <c r="E223" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="E223" s="2" t="s">
-        <v>538</v>
-      </c>
       <c r="F223" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H223" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="224" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5412,13 +5649,13 @@
         <v>5</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C224" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="E224" s="1" t="s">
         <v>525</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="225" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5426,13 +5663,13 @@
         <v>7</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C225" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="E225" s="2" t="s">
         <v>527</v>
-      </c>
-      <c r="E225" s="2" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="226" spans="1:12" ht="33" x14ac:dyDescent="0.25">
@@ -5440,10 +5677,10 @@
         <v>5</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="227" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5451,10 +5688,10 @@
         <v>7</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="228" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5462,22 +5699,22 @@
         <v>5</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C228" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D228" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="D228" s="1" t="s">
+      <c r="E228" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="E228" s="1" t="s">
+      <c r="F228" s="1" t="s">
         <v>515</v>
       </c>
-      <c r="F228" s="1" t="s">
+      <c r="L228" s="4" t="s">
         <v>516</v>
-      </c>
-      <c r="L228" s="4" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="229" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5485,22 +5722,22 @@
         <v>7</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C229" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="D229" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="D229" s="2" t="s">
+      <c r="E229" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="E229" s="2" t="s">
+      <c r="F229" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="F229" s="2" t="s">
+      <c r="L229" s="5" t="s">
         <v>521</v>
-      </c>
-      <c r="L229" s="5" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="230" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5508,13 +5745,13 @@
         <v>5</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C230" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D230" s="1" t="s">
         <v>509</v>
-      </c>
-      <c r="D230" s="1" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="231" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5522,13 +5759,13 @@
         <v>7</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C231" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="D231" s="5" t="s">
         <v>511</v>
-      </c>
-      <c r="D231" s="5" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="232" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5536,16 +5773,16 @@
         <v>5</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C232" t="s">
+        <v>503</v>
+      </c>
+      <c r="D232" t="s">
+        <v>502</v>
+      </c>
+      <c r="E232" s="1" t="s">
         <v>504</v>
-      </c>
-      <c r="D232" t="s">
-        <v>503</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="233" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5553,16 +5790,16 @@
         <v>7</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C233" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="D233" t="s">
+        <v>505</v>
+      </c>
+      <c r="E233" s="2" t="s">
         <v>507</v>
-      </c>
-      <c r="D233" t="s">
-        <v>506</v>
-      </c>
-      <c r="E233" s="2" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="234" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5570,19 +5807,19 @@
         <v>5</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C234" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D234" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="D234" s="1" t="s">
+      <c r="E234" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="E234" s="1" t="s">
+      <c r="F234" s="4" t="s">
         <v>497</v>
-      </c>
-      <c r="F234" s="4" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="235" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5590,19 +5827,19 @@
         <v>7</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E235" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F235" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="236" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5610,13 +5847,13 @@
         <v>5</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C236" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="D236" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="D236" s="1" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="237" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5624,13 +5861,13 @@
         <v>7</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C237" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="D237" s="2" t="s">
         <v>493</v>
-      </c>
-      <c r="D237" s="2" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="238" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5638,13 +5875,13 @@
         <v>5</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C238" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E238" s="1" t="s">
         <v>487</v>
-      </c>
-      <c r="E238" s="1" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="239" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5652,13 +5889,13 @@
         <v>7</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C239" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="E239" s="2" t="s">
         <v>489</v>
-      </c>
-      <c r="E239" s="2" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="240" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5666,13 +5903,13 @@
         <v>5</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D240" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="241" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -5680,13 +5917,13 @@
         <v>7</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="242" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -5694,16 +5931,16 @@
         <v>5</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C242" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="D242" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="E242" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="D242" s="4" t="s">
-        <v>477</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="243" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -5711,16 +5948,16 @@
         <v>7</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C243" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="D243" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="E243" s="2" t="s">
         <v>481</v>
-      </c>
-      <c r="D243" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="E243" s="2" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="244" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -5728,10 +5965,10 @@
         <v>5</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="245" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -5739,10 +5976,10 @@
         <v>7</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="246" spans="1:5" ht="33" x14ac:dyDescent="0.25">
@@ -5750,16 +5987,16 @@
         <v>5</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C246" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D246" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="D246" s="1" t="s">
+      <c r="E246" s="4" t="s">
         <v>470</v>
-      </c>
-      <c r="E246" s="4" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="247" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -5767,16 +6004,16 @@
         <v>7</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C247" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="D247" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="D247" s="2" t="s">
+      <c r="E247" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="E247" s="2" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="248" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -5784,16 +6021,16 @@
         <v>5</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C248" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="E248" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="D248" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="E248" s="1" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="249" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -5801,16 +6038,16 @@
         <v>7</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C249" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="D249" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="E249" s="2" t="s">
         <v>467</v>
-      </c>
-      <c r="D249" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="E249" s="2" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="250" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -5818,16 +6055,16 @@
         <v>5</v>
       </c>
       <c r="B250" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="E250" s="1" t="s">
         <v>456</v>
-      </c>
-      <c r="C250" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="D250" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="251" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -5835,16 +6072,16 @@
         <v>7</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C251" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="D251" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="D251" s="2" t="s">
-        <v>462</v>
-      </c>
       <c r="E251" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lorem Ipsum Generator running
Started instrumenting for Trace.

Created concept of WordList (ordered list of words)
</commit_message>
<xml_diff>
--- a/BasicTypes/Dictionary/RawData.xlsx
+++ b/BasicTypes/Dictionary/RawData.xlsx
@@ -2067,9 +2067,6 @@
     <t>disparagingly</t>
   </si>
   <si>
-    <t>monsuata</t>
-  </si>
-  <si>
     <t>fear, monster</t>
   </si>
   <si>
@@ -2281,6 +2278,9 @@
   </si>
   <si>
     <t>want</t>
+  </si>
+  <si>
+    <t>monsuta</t>
   </si>
 </sst>
 </file>
@@ -2665,8 +2665,8 @@
   <dimension ref="A1:N283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G141" sqref="G141"/>
+      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B282" sqref="B282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2730,13 +2730,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D2" t="s">
         <v>147</v>
       </c>
       <c r="F2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="L2" t="s">
         <v>3</v>
@@ -2914,7 +2914,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>31</v>
@@ -2941,7 +2941,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>36</v>
@@ -3132,13 +3132,13 @@
         <v>54</v>
       </c>
       <c r="D26" t="s">
+        <v>725</v>
+      </c>
+      <c r="E26" t="s">
         <v>726</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>727</v>
-      </c>
-      <c r="F26" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3160,13 +3160,13 @@
         <v>58</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>695</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>696</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3177,13 +3177,13 @@
         <v>58</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>699</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -3249,10 +3249,10 @@
         <v>70</v>
       </c>
       <c r="D32" t="s">
+        <v>728</v>
+      </c>
+      <c r="G32" t="s">
         <v>729</v>
-      </c>
-      <c r="G32" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -3450,7 +3450,7 @@
         <v>106</v>
       </c>
       <c r="D44" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -3549,7 +3549,7 @@
         <v>124</v>
       </c>
       <c r="D50" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3611,10 +3611,10 @@
         <v>135</v>
       </c>
       <c r="C54" t="s">
+        <v>733</v>
+      </c>
+      <c r="D54" t="s">
         <v>734</v>
-      </c>
-      <c r="D54" t="s">
-        <v>735</v>
       </c>
       <c r="E54" t="s">
         <v>136</v>
@@ -3648,7 +3648,7 @@
         <v>142</v>
       </c>
       <c r="D56" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -3847,7 +3847,7 @@
         <v>169</v>
       </c>
       <c r="C70" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D70" t="s">
         <v>171</v>
@@ -3986,7 +3986,7 @@
         <v>186</v>
       </c>
       <c r="E78" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4126,7 +4126,7 @@
         <v>206</v>
       </c>
       <c r="C88" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D88" t="s">
         <v>207</v>
@@ -4213,10 +4213,10 @@
         <v>218</v>
       </c>
       <c r="E94" t="s">
+        <v>737</v>
+      </c>
+      <c r="F94" t="s">
         <v>738</v>
-      </c>
-      <c r="F94" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
@@ -4238,19 +4238,19 @@
         <v>612</v>
       </c>
       <c r="C96" t="s">
+        <v>739</v>
+      </c>
+      <c r="D96" t="s">
         <v>740</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>741</v>
-      </c>
-      <c r="E96" t="s">
-        <v>742</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>614</v>
       </c>
       <c r="G96" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>613</v>
@@ -4421,7 +4421,7 @@
         <v>242</v>
       </c>
       <c r="D108" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="33" x14ac:dyDescent="0.25">
@@ -4570,7 +4570,7 @@
         <v>266</v>
       </c>
       <c r="G118" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="119" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -4629,13 +4629,13 @@
         <v>278</v>
       </c>
       <c r="C122" t="s">
+        <v>688</v>
+      </c>
+      <c r="E122" t="s">
         <v>689</v>
       </c>
-      <c r="E122" t="s">
+      <c r="F122" t="s">
         <v>690</v>
-      </c>
-      <c r="F122" t="s">
-        <v>691</v>
       </c>
       <c r="L122" s="1" t="s">
         <v>280</v>
@@ -4762,10 +4762,10 @@
         <v>302</v>
       </c>
       <c r="C130" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="D130" t="s">
         <v>746</v>
-      </c>
-      <c r="D130" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -4787,10 +4787,10 @@
         <v>304</v>
       </c>
       <c r="D132" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E132" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -4921,7 +4921,7 @@
         <v>320</v>
       </c>
       <c r="D142" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -4946,7 +4946,7 @@
         <v>324</v>
       </c>
       <c r="D144" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="145" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -4999,7 +4999,7 @@
         <v>330</v>
       </c>
       <c r="D148" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="149" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -5381,7 +5381,7 @@
         <v>395</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="175" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
@@ -5412,10 +5412,10 @@
         <v>399</v>
       </c>
       <c r="D176" t="s">
+        <v>704</v>
+      </c>
+      <c r="E176" s="1" t="s">
         <v>705</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="177" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5536,13 +5536,13 @@
         <v>603</v>
       </c>
       <c r="D184" t="s">
+        <v>706</v>
+      </c>
+      <c r="E184" t="s">
         <v>707</v>
       </c>
-      <c r="E184" t="s">
+      <c r="G184" t="s">
         <v>708</v>
-      </c>
-      <c r="G184" t="s">
-        <v>709</v>
       </c>
       <c r="H184" s="1" t="s">
         <v>604</v>
@@ -5607,10 +5607,10 @@
         <v>595</v>
       </c>
       <c r="D188" t="s">
+        <v>723</v>
+      </c>
+      <c r="E188" t="s">
         <v>724</v>
-      </c>
-      <c r="E188" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="189" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -5635,13 +5635,13 @@
         <v>593</v>
       </c>
       <c r="D190" t="s">
+        <v>701</v>
+      </c>
+      <c r="F190" t="s">
         <v>702</v>
       </c>
-      <c r="F190" t="s">
+      <c r="G190" t="s">
         <v>703</v>
-      </c>
-      <c r="G190" t="s">
-        <v>704</v>
       </c>
       <c r="I190" s="1" t="s">
         <v>593</v>
@@ -5725,7 +5725,7 @@
         <v>584</v>
       </c>
       <c r="E196" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="197" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -5815,7 +5815,7 @@
         <v>574</v>
       </c>
       <c r="D202" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="203" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -5840,7 +5840,7 @@
         <v>570</v>
       </c>
       <c r="D204" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>571</v>
@@ -5939,7 +5939,7 @@
         <v>555</v>
       </c>
       <c r="G210" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="211" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -5970,10 +5970,10 @@
         <v>552</v>
       </c>
       <c r="D212" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="G212" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="213" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -6026,7 +6026,7 @@
         <v>546</v>
       </c>
       <c r="G216" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="217" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -6085,7 +6085,7 @@
         <v>536</v>
       </c>
       <c r="G220" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="M220" t="s">
         <v>537</v>
@@ -6162,7 +6162,7 @@
         <v>522</v>
       </c>
       <c r="D224" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E224" s="1" t="s">
         <v>523</v>
@@ -6193,7 +6193,7 @@
         <v>520</v>
       </c>
       <c r="E226" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="227" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -6369,7 +6369,7 @@
         <v>489</v>
       </c>
       <c r="E236" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="237" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
@@ -6428,7 +6428,7 @@
         <v>480</v>
       </c>
       <c r="E240" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="241" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -6490,7 +6490,7 @@
         <v>472</v>
       </c>
       <c r="D244" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="245" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -6589,7 +6589,7 @@
         <v>454</v>
       </c>
       <c r="F250" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="251" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -6620,7 +6620,7 @@
         <v>315</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="253" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
@@ -7001,22 +7001,22 @@
         <v>5</v>
       </c>
       <c r="B282" t="s">
+        <v>754</v>
+      </c>
+      <c r="C282" t="s">
         <v>683</v>
       </c>
-      <c r="C282" t="s">
+      <c r="D282" t="s">
         <v>684</v>
       </c>
-      <c r="D282" t="s">
+      <c r="E282" t="s">
         <v>685</v>
       </c>
-      <c r="E282" t="s">
+      <c r="F282" t="s">
         <v>686</v>
       </c>
-      <c r="F282" t="s">
+      <c r="G282" t="s">
         <v>687</v>
-      </c>
-      <c r="G282" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.25">
@@ -7024,7 +7024,7 @@
         <v>7</v>
       </c>
       <c r="B283" t="s">
-        <v>683</v>
+        <v>754</v>
       </c>
     </row>
   </sheetData>

</xml_diff>